<commit_message>
week 12 session 2
</commit_message>
<xml_diff>
--- a/regression materials/softserve scatter.xlsx
+++ b/regression materials/softserve scatter.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tn9k4\GitHub\courses_teach\mizzou\mar4050_F21\regression materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tn9k4\GitHub\courses_teach\mizzou\mar4050_S22\regression materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F73580-18F3-4BE9-A98D-C5DE3D792A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292C9A80-E998-46B1-B87C-8C7D021954B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="regression" sheetId="4" r:id="rId1"/>
+    <sheet name="correlation" sheetId="6" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>no regression line</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>Upper 95.0%</t>
-  </si>
-  <si>
-    <t>X Variable 1</t>
   </si>
 </sst>
 </file>
@@ -1572,11 +1569,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DAA3C8-4B70-4EEC-A5C6-6FF4CF9ED488}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A927F12-7FB0-4A81-90FC-718E23F8A7C5}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1768,7 +1765,7 @@
     </row>
     <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B18" s="3">
         <v>0.11640596722915131</v>
@@ -1802,228 +1799,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75B73735-9945-43E8-8ED2-07FDEE71CE3B}">
-  <dimension ref="A1:I18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB0D56E-0FC5-47C6-BABE-10602BAD14D1}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.80209490427016672</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.64335623545616794</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.62784998482382737</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1.6342798997776842</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="2">
-        <v>110.8147558112008</v>
-      </c>
-      <c r="D12" s="2">
-        <v>110.8147558112008</v>
-      </c>
-      <c r="E12" s="2">
-        <v>41.490122319727995</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1.4244453127205321E-6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2">
-        <v>23</v>
-      </c>
-      <c r="C13" s="2">
-        <v>61.430028188799213</v>
-      </c>
-      <c r="D13" s="2">
-        <v>2.6708707908173572</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3">
-        <v>24</v>
-      </c>
-      <c r="C14" s="3">
-        <v>172.24478400000001</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="2">
-        <v>-1.3057479090242072</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0.98813262661607248</v>
-      </c>
-      <c r="D17" s="2">
-        <v>-1.3214298099798909</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.19935318942045022</v>
-      </c>
-      <c r="F17" s="2">
-        <v>-3.3498559871769102</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0.73836016912849578</v>
-      </c>
-      <c r="H17" s="2">
-        <v>-3.3498559871769102</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0.73836016912849578</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="3">
-        <v>0.11640596722915131</v>
-      </c>
-      <c r="C18" s="3">
-        <v>1.8071861359662319E-2</v>
-      </c>
-      <c r="D18" s="3">
-        <v>6.4412826610643279</v>
-      </c>
-      <c r="E18" s="3">
-        <v>1.4244453127205425E-6</v>
-      </c>
-      <c r="F18" s="3">
-        <v>7.9021473693047906E-2</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0.15379046076525471</v>
-      </c>
-      <c r="H18" s="3">
-        <v>7.9021473693047906E-2</v>
-      </c>
-      <c r="I18" s="3">
-        <v>0.15379046076525471</v>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.80209490427016683</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2036,7 +1847,7 @@
   <dimension ref="A4:B68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>